<commit_message>
cast get pit stop time to float
</commit_message>
<xml_diff>
--- a/analysis/data/out.xlsx
+++ b/analysis/data/out.xlsx
@@ -930,11 +930,8 @@
       <c r="D20" t="n">
         <v>167.633</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>5557    31.336
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E20" t="n">
+        <v>31.336</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -2758,11 +2755,8 @@
       <c r="D93" t="n">
         <v>110.632</v>
       </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>5558    22.293
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E93" t="n">
+        <v>22.293</v>
       </c>
       <c r="F93" t="n">
         <v>383.372</v>
@@ -4811,11 +4805,8 @@
       <c r="D175" t="n">
         <v>128.894</v>
       </c>
-      <c r="E175" t="inlineStr">
-        <is>
-          <t>5559    39.562
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E175" t="n">
+        <v>39.562</v>
       </c>
       <c r="F175" t="n">
         <v>760.198</v>
@@ -7689,11 +7680,8 @@
       <c r="D290" t="n">
         <v>108.477</v>
       </c>
-      <c r="E290" t="inlineStr">
-        <is>
-          <t>5560    22.154
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E290" t="n">
+        <v>22.154</v>
       </c>
       <c r="F290" t="n">
         <v>1295.109</v>
@@ -7742,11 +7730,8 @@
       <c r="D292" t="n">
         <v>116.702</v>
       </c>
-      <c r="E292" t="inlineStr">
-        <is>
-          <t>5561    28.591
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E292" t="n">
+        <v>28.591</v>
       </c>
       <c r="F292" t="n">
         <v>1318.177</v>
@@ -8120,11 +8105,8 @@
       <c r="D307" t="n">
         <v>109.469</v>
       </c>
-      <c r="E307" t="inlineStr">
-        <is>
-          <t>5562    22.484
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E307" t="n">
+        <v>22.484</v>
       </c>
       <c r="F307" t="n">
         <v>1382.849</v>
@@ -8148,11 +8130,8 @@
       <c r="D308" t="n">
         <v>109.892</v>
       </c>
-      <c r="E308" t="inlineStr">
-        <is>
-          <t>5563    23.13
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E308" t="n">
+        <v>23.13</v>
       </c>
       <c r="F308" t="n">
         <v>1384.382</v>
@@ -8276,11 +8255,8 @@
       <c r="D313" t="n">
         <v>106.345</v>
       </c>
-      <c r="E313" t="inlineStr">
-        <is>
-          <t>5564    21.709
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E313" t="n">
+        <v>21.709</v>
       </c>
       <c r="F313" t="n">
         <v>1424.777</v>
@@ -8529,11 +8505,8 @@
       <c r="D323" t="n">
         <v>108.359</v>
       </c>
-      <c r="E323" t="inlineStr">
-        <is>
-          <t>5565    22.045
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E323" t="n">
+        <v>22.045</v>
       </c>
       <c r="F323" t="n">
         <v>1463.649</v>
@@ -8957,11 +8930,8 @@
       <c r="D340" t="n">
         <v>107.439</v>
       </c>
-      <c r="E340" t="inlineStr">
-        <is>
-          <t>5566    21.762
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E340" t="n">
+        <v>21.762</v>
       </c>
       <c r="F340" t="n">
         <v>1552.844</v>
@@ -9785,11 +9755,8 @@
       <c r="D373" t="n">
         <v>107.482</v>
       </c>
-      <c r="E373" t="inlineStr">
-        <is>
-          <t>5567    21.568
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E373" t="n">
+        <v>21.568</v>
       </c>
       <c r="F373" t="n">
         <v>1728.14</v>
@@ -10963,11 +10930,8 @@
       <c r="D420" t="n">
         <v>106.995</v>
       </c>
-      <c r="E420" t="inlineStr">
-        <is>
-          <t>5568    21.988
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E420" t="n">
+        <v>21.988</v>
       </c>
       <c r="F420" t="n">
         <v>1956.362</v>
@@ -11816,11 +11780,8 @@
       <c r="D454" t="n">
         <v>106.647</v>
       </c>
-      <c r="E454" t="inlineStr">
-        <is>
-          <t>5569    21.44
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E454" t="n">
+        <v>21.44</v>
       </c>
       <c r="F454" t="n">
         <v>2146.56</v>
@@ -11894,11 +11855,8 @@
       <c r="D457" t="n">
         <v>108.655</v>
       </c>
-      <c r="E457" t="inlineStr">
-        <is>
-          <t>5570    22.208
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E457" t="n">
+        <v>22.208</v>
       </c>
       <c r="F457" t="n">
         <v>2159.527</v>
@@ -12247,11 +12205,8 @@
       <c r="D471" t="n">
         <v>106.225</v>
       </c>
-      <c r="E471" t="inlineStr">
-        <is>
-          <t>5571    22.033
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E471" t="n">
+        <v>22.033</v>
       </c>
       <c r="F471" t="n">
         <v>2241.266000000001</v>
@@ -13875,11 +13830,8 @@
       <c r="D536" t="n">
         <v>110.755</v>
       </c>
-      <c r="E536" t="inlineStr">
-        <is>
-          <t>5572    22.38
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E536" t="n">
+        <v>22.38</v>
       </c>
       <c r="F536" t="n">
         <v>2594.589</v>
@@ -14253,11 +14205,8 @@
       <c r="D551" t="n">
         <v>110.816</v>
       </c>
-      <c r="E551" t="inlineStr">
-        <is>
-          <t>5573    23.159
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E551" t="n">
+        <v>23.159</v>
       </c>
       <c r="F551" t="n">
         <v>2682.397999999999</v>
@@ -15631,11 +15580,8 @@
       <c r="D606" t="n">
         <v>111.432</v>
       </c>
-      <c r="E606" t="inlineStr">
-        <is>
-          <t>5574    25.559
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E606" t="n">
+        <v>25.559</v>
       </c>
       <c r="F606" t="n">
         <v>2995.086</v>
@@ -20209,11 +20155,8 @@
       <c r="D789" t="n">
         <v>110.882</v>
       </c>
-      <c r="E789" t="inlineStr">
-        <is>
-          <t>5575    22.189
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E789" t="n">
+        <v>22.189</v>
       </c>
       <c r="F789" t="n">
         <v>4031.244</v>
@@ -21487,11 +21430,8 @@
       <c r="D840" t="n">
         <v>109.074</v>
       </c>
-      <c r="E840" t="inlineStr">
-        <is>
-          <t>5576    24.026
-Name: milliseconds, dtype: float64</t>
-        </is>
+      <c r="E840" t="n">
+        <v>24.026</v>
       </c>
       <c r="F840" t="n">
         <v>4354.535999999998</v>

</xml_diff>